<commit_message>
screen -> render2d, view -> render3d
</commit_message>
<xml_diff>
--- a/docs/Game Binary Size Tracking.xlsx
+++ b/docs/Game Binary Size Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B417427B-CBE3-4015-8EC3-47C5BBDE8D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E2FBFC-6F40-47F4-B3C1-C25C0AF1A069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Debug" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>gamex64</t>
   </si>
@@ -140,6 +140,39 @@
   </si>
   <si>
     <t>Remove vulkan renderer</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 3</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 4</t>
+  </si>
+  <si>
+    <t>v0.0.4, prerelease 5</t>
+  </si>
+  <si>
+    <t>v0.0.4</t>
+  </si>
+  <si>
+    <t>v0.0.5</t>
+  </si>
+  <si>
+    <t>v0.0.6.9 (post-Curl)</t>
+  </si>
+  <si>
+    <t>v0.0.6.47 (pre-GLFW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v0.0.6.161 </t>
+  </si>
+  <si>
+    <t>v0.0.7.299</t>
+  </si>
+  <si>
+    <t>v0.0.8.377</t>
+  </si>
+  <si>
+    <t>v0.0.9.480</t>
   </si>
 </sst>
 </file>
@@ -495,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A747356-481A-4057-AC51-1B21755F8FCB}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,10 +1380,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D702C5CE-747D-4EE4-B54A-F08904BF5F33}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1442,7 @@
         <v>147456</v>
       </c>
       <c r="E2">
-        <f>B2+C2+D2</f>
+        <f t="shared" ref="E2:E16" si="0">B2+C2+D2</f>
         <v>1338880</v>
       </c>
       <c r="G2" s="2"/>
@@ -1431,7 +1464,7 @@
         <v>147456</v>
       </c>
       <c r="E3">
-        <f>B3+C3+D3</f>
+        <f t="shared" si="0"/>
         <v>1338368</v>
       </c>
       <c r="G3" s="2"/>
@@ -1453,7 +1486,7 @@
         <v>147456</v>
       </c>
       <c r="E4">
-        <f>B4+C4+D4</f>
+        <f t="shared" si="0"/>
         <v>1336320</v>
       </c>
       <c r="I4" t="s">
@@ -1474,7 +1507,7 @@
         <v>147456</v>
       </c>
       <c r="E5">
-        <f>B5+C5+D5</f>
+        <f t="shared" si="0"/>
         <v>1340416</v>
       </c>
       <c r="I5" t="s">
@@ -1482,62 +1515,294 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>45305.894444444442</v>
+      </c>
+      <c r="B6">
+        <v>923136</v>
+      </c>
+      <c r="C6">
+        <v>255488</v>
+      </c>
+      <c r="D6">
+        <v>148480</v>
+      </c>
       <c r="E6">
-        <f>B6+C6+D6</f>
+        <f t="shared" si="0"/>
+        <v>1327104</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>45332.685416666667</v>
+      </c>
+      <c r="B7">
+        <v>923136</v>
+      </c>
+      <c r="C7">
+        <v>274944</v>
+      </c>
+      <c r="D7">
+        <v>147968</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1346048</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>45344.85</v>
+      </c>
+      <c r="B8">
+        <v>940032</v>
+      </c>
+      <c r="C8">
+        <v>275456</v>
+      </c>
+      <c r="D8">
+        <v>149504</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1364992</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45361.917361111111</v>
+      </c>
+      <c r="B9">
+        <v>943104</v>
+      </c>
+      <c r="C9">
+        <v>277504</v>
+      </c>
+      <c r="D9">
+        <v>148480</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1369088</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45374.79583333333</v>
+      </c>
+      <c r="B10">
+        <v>950784</v>
+      </c>
+      <c r="C10">
+        <v>278016</v>
+      </c>
+      <c r="D10">
+        <v>147456</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>1376256</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45377.929166666669</v>
+      </c>
+      <c r="B11">
+        <v>1444864</v>
+      </c>
+      <c r="C11">
+        <v>278016</v>
+      </c>
+      <c r="D11">
+        <v>147456</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1870336</v>
+      </c>
+      <c r="I11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45382.916666666664</v>
+      </c>
+      <c r="B12">
+        <v>1445376</v>
+      </c>
+      <c r="C12">
+        <v>258560</v>
+      </c>
+      <c r="D12">
+        <v>147456</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>1851392</v>
+      </c>
+      <c r="I12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45388.847916666666</v>
+      </c>
+      <c r="B13">
+        <v>1442816</v>
+      </c>
+      <c r="C13">
+        <v>259072</v>
+      </c>
+      <c r="D13">
+        <v>334848</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>2036736</v>
+      </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45402.642361111109</v>
+      </c>
+      <c r="B14">
+        <v>1425408</v>
+      </c>
+      <c r="C14">
+        <v>257536</v>
+      </c>
+      <c r="D14">
+        <v>336384</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>2019328</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45416.893055555556</v>
+      </c>
+      <c r="B15">
+        <v>1425408</v>
+      </c>
+      <c r="C15">
+        <v>257024</v>
+      </c>
+      <c r="D15">
+        <v>336384</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>2018816</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45437.818749999999</v>
+      </c>
+      <c r="B16">
+        <v>1412096</v>
+      </c>
+      <c r="C16">
+        <v>257536</v>
+      </c>
+      <c r="D16">
+        <v>335872</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2005504</v>
+      </c>
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="E17">
+        <f t="shared" ref="E17:E26" si="1">B17+C17+D17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <f>B7+C7+D7</f>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E8">
-        <f>B8+C8+D8</f>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E9">
-        <f>B9+C9+D9</f>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <f>B10+C10+D10</f>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11">
-        <f>B11+C11+D11</f>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12">
-        <f>B12+C12+D12</f>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <f>B13+C13+D13</f>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14">
-        <f>B14+C14+D14</f>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15">
-        <f>B15+C15+D15</f>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.1-pre1 final + add release generation tool
</commit_message>
<xml_diff>
--- a/docs/Game Binary Size Tracking.xlsx
+++ b/docs/Game Binary Size Tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA2E20D-EB7E-48B4-8C1E-383F09831143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5D320E-EF92-4BF0-B046-C5FA7A9ECE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B3D47C4B-CC62-4480-B329-FB279CE950D6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>gamex64</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>v0.0.10.553</t>
+  </si>
+  <si>
+    <t>v0.1.0.656 (v0.1.0, prerelease 1) RC1</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1389,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1402,7 @@
     <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1770,9 +1773,24 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45472.625694444447</v>
+      </c>
+      <c r="B18">
+        <v>1438720</v>
+      </c>
+      <c r="C18">
+        <v>259584</v>
+      </c>
+      <c r="D18">
+        <v>337408</v>
+      </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2035712</v>
+      </c>
+      <c r="I18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>